<commit_message>
New concept graphic for wiki
</commit_message>
<xml_diff>
--- a/Documentation/Concept Flow Diagram.xlsx
+++ b/Documentation/Concept Flow Diagram.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="14370"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="14370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$C$2:$M$26</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Accepts player connections and routes messages</t>
   </si>
@@ -56,12 +59,30 @@
   <si>
     <t>Serialisation is to SQL database. Cache provides faster access to recently used data.</t>
   </si>
+  <si>
+    <t>MySQL Cluster / Oracle</t>
+  </si>
+  <si>
+    <t>Region Data Processor</t>
+  </si>
+  <si>
+    <t>Player Handler</t>
+  </si>
+  <si>
+    <t>World Controller</t>
+  </si>
+  <si>
+    <t>AI/Environment</t>
+  </si>
+  <si>
+    <t>Connection Handler</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,16 +90,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -86,14 +119,185 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1511,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="L4:P32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Y35"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1590,13 +1794,350 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="C1:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N27" sqref="B1:N27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="1.7109375" style="1" customWidth="1"/>
+    <col min="3" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="1.7109375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:15" ht="9" customHeight="1" thickBot="1"/>
+    <row r="2" spans="3:15" ht="15.75" thickTop="1">
+      <c r="C2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="3:15">
+      <c r="C3" s="13"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" spans="3:15" ht="15.75" thickBot="1">
+      <c r="C4" s="13"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="3:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C5" s="4"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="4"/>
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="3:15" ht="15.75" thickTop="1">
+      <c r="C6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="G6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
+      <c r="K6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="11"/>
+      <c r="M6" s="12"/>
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="3:15">
+      <c r="C7" s="13"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="14"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="14"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="14"/>
+      <c r="N7"/>
+    </row>
+    <row r="8" spans="3:15" ht="15.75" thickBot="1">
+      <c r="C8" s="15"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="17"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="17"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="17"/>
+      <c r="N8"/>
+    </row>
+    <row r="9" spans="3:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="N9"/>
+    </row>
+    <row r="10" spans="3:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="7"/>
+      <c r="N10"/>
+    </row>
+    <row r="11" spans="3:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="H11" s="2"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+    </row>
+    <row r="12" spans="3:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="12"/>
+      <c r="F12"/>
+      <c r="G12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+    </row>
+    <row r="13" spans="3:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C13" s="13"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="25"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+    </row>
+    <row r="14" spans="3:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+      <c r="F14"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="17"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+    </row>
+    <row r="15" spans="3:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="H15" s="22"/>
+      <c r="I15" s="9"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="3:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C16"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="8"/>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="3:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C17" s="21"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="3"/>
+      <c r="L17" s="2"/>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="3:13" ht="15.75" thickTop="1">
+      <c r="C18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="14"/>
+      <c r="G18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="14"/>
+      <c r="K18" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18" s="12"/>
+    </row>
+    <row r="19" spans="3:13">
+      <c r="C19" s="13"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="14"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="14"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="14"/>
+    </row>
+    <row r="20" spans="3:13" ht="15.75" thickBot="1">
+      <c r="C20" s="13"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="14"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="14"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="17"/>
+    </row>
+    <row r="21" spans="3:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="C21" s="24"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="3:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="7"/>
+    </row>
+    <row r="23" spans="3:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="4"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+    </row>
+    <row r="24" spans="3:13" ht="15.75" thickTop="1">
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="11"/>
+      <c r="I24" s="14"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+    </row>
+    <row r="25" spans="3:13">
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="14"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+    </row>
+    <row r="26" spans="3:13" ht="15.75" thickBot="1">
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="3:13" ht="9" customHeight="1" thickTop="1"/>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="C18:E20"/>
+    <mergeCell ref="G18:I20"/>
+    <mergeCell ref="G24:I26"/>
+    <mergeCell ref="C2:M4"/>
+    <mergeCell ref="G12:I14"/>
+    <mergeCell ref="K18:M20"/>
+    <mergeCell ref="C6:E8"/>
+    <mergeCell ref="G6:I8"/>
+    <mergeCell ref="K6:M8"/>
+    <mergeCell ref="C12:E14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Removed AI from graphic, realised give the region processors something to do
</commit_message>
<xml_diff>
--- a/Documentation/Concept Flow Diagram.xlsx
+++ b/Documentation/Concept Flow Diagram.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$C$2:$M$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$B$1:$N$27</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Accepts player connections and routes messages</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>World Controller</t>
-  </si>
-  <si>
-    <t>AI/Environment</t>
   </si>
   <si>
     <t>Connection Handler</t>
@@ -226,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -295,6 +292,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1797,7 +1796,7 @@
   <dimension ref="C1:O27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="B1:N27"/>
+      <selection activeCell="B1" sqref="B1:N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1937,12 +1936,10 @@
       <c r="N11"/>
       <c r="O11"/>
     </row>
-    <row r="12" spans="3:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="12"/>
+    <row r="12" spans="3:15" ht="15.75" thickTop="1">
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
       <c r="F12"/>
       <c r="G12" s="10" t="s">
         <v>16</v>
@@ -1956,11 +1953,11 @@
       <c r="N12"/>
       <c r="O12"/>
     </row>
-    <row r="13" spans="3:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C13" s="13"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="6"/>
+    <row r="13" spans="3:15">
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -1971,10 +1968,10 @@
       <c r="N13"/>
       <c r="O13"/>
     </row>
-    <row r="14" spans="3:15" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
+    <row r="14" spans="3:15" ht="15.75" thickBot="1">
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
       <c r="F14"/>
       <c r="G14" s="15"/>
       <c r="H14" s="11"/>
@@ -2095,7 +2092,7 @@
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="14"/>
@@ -2124,7 +2121,7 @@
     </row>
     <row r="27" spans="3:13" ht="9" customHeight="1" thickTop="1"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="C18:E20"/>
     <mergeCell ref="G18:I20"/>
     <mergeCell ref="G24:I26"/>
@@ -2134,7 +2131,6 @@
     <mergeCell ref="C6:E8"/>
     <mergeCell ref="G6:I8"/>
     <mergeCell ref="K6:M8"/>
-    <mergeCell ref="C12:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>